<commit_message>
14 05 2023 1
</commit_message>
<xml_diff>
--- a/openvariantfipi/1_18.xlsx
+++ b/openvariantfipi/1_18.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="360" windowWidth="28515" windowHeight="12315"/>
+    <workbookView xWindow="240" yWindow="360" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,75 +1814,75 @@
         <v>51</v>
       </c>
       <c r="B23" s="15">
-        <f>MIN(A23,B22)+B2</f>
+        <f t="shared" ref="B23:S23" si="1">MIN(A23,B22)+B2</f>
         <v>123</v>
       </c>
       <c r="C23" s="15">
-        <f>MIN(B23,C22)+C2</f>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
       <c r="D23" s="15">
-        <f>MIN(C23,D22)+D2</f>
+        <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="E23" s="15">
-        <f>MIN(D23,E22)+E2</f>
+        <f t="shared" si="1"/>
         <v>214</v>
       </c>
       <c r="F23" s="15">
-        <f>MIN(E23,F22)+F2</f>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
       <c r="G23" s="15">
-        <f>MIN(F23,G22)+G2</f>
+        <f t="shared" si="1"/>
         <v>296</v>
       </c>
       <c r="H23" s="15">
-        <f>MIN(G23,H22)+H2</f>
+        <f t="shared" si="1"/>
         <v>373</v>
       </c>
       <c r="I23" s="15">
-        <f>MIN(H23,I22)+I2</f>
+        <f t="shared" si="1"/>
         <v>396</v>
       </c>
       <c r="J23" s="15">
-        <f>MIN(I23,J22)+J2</f>
+        <f t="shared" si="1"/>
         <v>428</v>
       </c>
       <c r="K23" s="15">
-        <f>MIN(J23,K22)+K2</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="L23" s="15">
-        <f>MIN(K23,L22)+L2</f>
+        <f t="shared" si="1"/>
         <v>547</v>
       </c>
       <c r="M23" s="15">
-        <f>MIN(L23,M22)+M2</f>
+        <f t="shared" si="1"/>
         <v>562</v>
       </c>
       <c r="N23" s="15">
-        <f>MIN(M23,N22)+N2</f>
+        <f t="shared" si="1"/>
         <v>582</v>
       </c>
       <c r="O23" s="15">
-        <f>MIN(N23,O22)+O2</f>
+        <f t="shared" si="1"/>
         <v>638</v>
       </c>
       <c r="P23" s="15">
-        <f>MIN(O23,P22)+P2</f>
+        <f t="shared" si="1"/>
         <v>692</v>
       </c>
       <c r="Q23" s="15">
-        <f>MIN(P23,Q22)+Q2</f>
+        <f t="shared" si="1"/>
         <v>769</v>
       </c>
       <c r="R23" s="15">
-        <f>MIN(Q23,R22)+R2</f>
+        <f t="shared" si="1"/>
         <v>796</v>
       </c>
       <c r="S23" s="16">
-        <f>MIN(R23,S22)+S2</f>
+        <f t="shared" si="1"/>
         <v>812</v>
       </c>
       <c r="T23" s="17">
@@ -1892,7 +1892,7 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <f t="shared" ref="A24:A40" si="1">A23+A3</f>
+        <f t="shared" ref="A24:A40" si="2">A23+A3</f>
         <v>62</v>
       </c>
       <c r="B24" s="18">
@@ -1900,81 +1900,81 @@
         <v>92</v>
       </c>
       <c r="C24" s="18">
-        <f t="shared" ref="C24:F24" si="2">B24+C3</f>
+        <f t="shared" ref="C24:F24" si="3">B24+C3</f>
         <v>172</v>
       </c>
       <c r="D24" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>192</v>
       </c>
       <c r="E24" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="F24" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>212</v>
       </c>
       <c r="G24" s="15">
-        <f>MIN(F24,G23)+G3</f>
+        <f t="shared" ref="G24:S25" si="4">MIN(F24,G23)+G3</f>
         <v>280</v>
       </c>
       <c r="H24" s="15">
-        <f>MIN(G24,H23)+H3</f>
+        <f t="shared" si="4"/>
         <v>343</v>
       </c>
       <c r="I24" s="15">
-        <f>MIN(H24,I23)+I3</f>
+        <f t="shared" si="4"/>
         <v>408</v>
       </c>
       <c r="J24" s="15">
-        <f>MIN(I24,J23)+J3</f>
+        <f t="shared" si="4"/>
         <v>432</v>
       </c>
       <c r="K24" s="15">
-        <f>MIN(J24,K23)+K3</f>
+        <f t="shared" si="4"/>
         <v>459</v>
       </c>
       <c r="L24" s="15">
-        <f>MIN(K24,L23)+L3</f>
+        <f t="shared" si="4"/>
         <v>479</v>
       </c>
       <c r="M24" s="15">
-        <f>MIN(L24,M23)+M3</f>
+        <f t="shared" si="4"/>
         <v>517</v>
       </c>
       <c r="N24" s="15">
-        <f>MIN(M24,N23)+N3</f>
+        <f t="shared" si="4"/>
         <v>596</v>
       </c>
       <c r="O24" s="15">
-        <f>MIN(N24,O23)+O3</f>
+        <f t="shared" si="4"/>
         <v>677</v>
       </c>
       <c r="P24" s="15">
-        <f>MIN(O24,P23)+P3</f>
+        <f t="shared" si="4"/>
         <v>762</v>
       </c>
       <c r="Q24" s="15">
-        <f>MIN(P24,Q23)+Q3</f>
+        <f t="shared" si="4"/>
         <v>812</v>
       </c>
       <c r="R24" s="15">
-        <f>MIN(Q24,R23)+R3</f>
+        <f t="shared" si="4"/>
         <v>861</v>
       </c>
       <c r="S24" s="16">
-        <f>MIN(R24,S23)+S3</f>
+        <f t="shared" si="4"/>
         <v>859</v>
       </c>
       <c r="T24" s="17">
-        <f t="shared" ref="T24:T30" si="3">T23+T3</f>
+        <f t="shared" ref="T24:T30" si="5">T23+T3</f>
         <v>944</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="B25" s="15"/>
@@ -1995,81 +1995,81 @@
         <v>290</v>
       </c>
       <c r="G25" s="15">
-        <f>MIN(F25,G24)+G4</f>
+        <f t="shared" si="4"/>
         <v>308</v>
       </c>
       <c r="H25" s="15">
-        <f>MIN(G25,H24)+H4</f>
+        <f t="shared" si="4"/>
         <v>318</v>
       </c>
       <c r="I25" s="15">
-        <f>MIN(H25,I24)+I4</f>
+        <f t="shared" si="4"/>
         <v>383</v>
       </c>
       <c r="J25" s="15">
-        <f>MIN(I25,J24)+J4</f>
+        <f t="shared" si="4"/>
         <v>407</v>
       </c>
       <c r="K25" s="15">
-        <f>MIN(J25,K24)+K4</f>
+        <f t="shared" si="4"/>
         <v>432</v>
       </c>
       <c r="L25" s="15">
-        <f>MIN(K25,L24)+L4</f>
+        <f t="shared" si="4"/>
         <v>461</v>
       </c>
       <c r="M25" s="15">
-        <f>MIN(L25,M24)+M4</f>
+        <f t="shared" si="4"/>
         <v>510</v>
       </c>
       <c r="N25" s="15">
-        <f>MIN(M25,N24)+N4</f>
+        <f t="shared" si="4"/>
         <v>577</v>
       </c>
       <c r="O25" s="15">
-        <f>MIN(N25,O24)+O4</f>
+        <f t="shared" si="4"/>
         <v>658</v>
       </c>
       <c r="P25" s="15">
-        <f>MIN(O25,P24)+P4</f>
+        <f t="shared" si="4"/>
         <v>743</v>
       </c>
       <c r="Q25" s="15">
-        <f>MIN(P25,Q24)+Q4</f>
+        <f t="shared" si="4"/>
         <v>798</v>
       </c>
       <c r="R25" s="15">
-        <f>MIN(Q25,R24)+R4</f>
+        <f t="shared" si="4"/>
         <v>834</v>
       </c>
       <c r="S25" s="16">
-        <f>MIN(R25,S24)+S4</f>
+        <f t="shared" si="4"/>
         <v>904</v>
       </c>
       <c r="T25" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>963</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119</v>
       </c>
       <c r="B26" s="15">
-        <f>MIN(A26,B25)+B5</f>
+        <f t="shared" ref="B26:E27" si="6">MIN(A26,B25)+B5</f>
         <v>194</v>
       </c>
       <c r="C26" s="15">
-        <f>MIN(B26,C25)+C5</f>
+        <f t="shared" si="6"/>
         <v>226</v>
       </c>
       <c r="D26" s="15">
-        <f>MIN(C26,D25)+D5</f>
+        <f t="shared" si="6"/>
         <v>257</v>
       </c>
       <c r="E26" s="15">
-        <f>MIN(D26,E25)+E5</f>
+        <f t="shared" si="6"/>
         <v>284</v>
       </c>
       <c r="F26" s="18">
@@ -2077,81 +2077,81 @@
         <v>324</v>
       </c>
       <c r="G26" s="18">
-        <f t="shared" ref="G26:J26" si="4">F26+G5</f>
+        <f t="shared" ref="G26:J26" si="7">F26+G5</f>
         <v>354</v>
       </c>
       <c r="H26" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>399</v>
       </c>
       <c r="I26" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>426</v>
       </c>
       <c r="J26" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>470</v>
       </c>
       <c r="K26" s="15">
-        <f>MIN(J26,K25)+K5</f>
+        <f t="shared" ref="K26:S27" si="8">MIN(J26,K25)+K5</f>
         <v>441</v>
       </c>
       <c r="L26" s="15">
-        <f>MIN(K26,L25)+L5</f>
+        <f t="shared" si="8"/>
         <v>453</v>
       </c>
       <c r="M26" s="15">
-        <f>MIN(L26,M25)+M5</f>
+        <f t="shared" si="8"/>
         <v>522</v>
       </c>
       <c r="N26" s="15">
-        <f>MIN(M26,N25)+N5</f>
+        <f t="shared" si="8"/>
         <v>603</v>
       </c>
       <c r="O26" s="15">
-        <f>MIN(N26,O25)+O5</f>
+        <f t="shared" si="8"/>
         <v>678</v>
       </c>
       <c r="P26" s="15">
-        <f>MIN(O26,P25)+P5</f>
+        <f t="shared" si="8"/>
         <v>741</v>
       </c>
       <c r="Q26" s="15">
-        <f>MIN(P26,Q25)+Q5</f>
+        <f t="shared" si="8"/>
         <v>820</v>
       </c>
       <c r="R26" s="15">
-        <f>MIN(Q26,R25)+R5</f>
+        <f t="shared" si="8"/>
         <v>876</v>
       </c>
       <c r="S26" s="16">
-        <f>MIN(R26,S25)+S5</f>
+        <f t="shared" si="8"/>
         <v>918</v>
       </c>
       <c r="T26" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1011</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="B27" s="15">
-        <f>MIN(A27,B26)+B6</f>
+        <f t="shared" si="6"/>
         <v>208</v>
       </c>
       <c r="C27" s="15">
-        <f>MIN(B27,C26)+C6</f>
+        <f t="shared" si="6"/>
         <v>225</v>
       </c>
       <c r="D27" s="15">
-        <f>MIN(C27,D26)+D6</f>
+        <f t="shared" si="6"/>
         <v>275</v>
       </c>
       <c r="E27" s="15">
-        <f>MIN(D27,E26)+E6</f>
+        <f t="shared" si="6"/>
         <v>281</v>
       </c>
       <c r="F27" s="15">
@@ -2175,61 +2175,61 @@
         <v>372</v>
       </c>
       <c r="K27" s="15">
-        <f>MIN(J27,K26)+K6</f>
+        <f t="shared" si="8"/>
         <v>383</v>
       </c>
       <c r="L27" s="15">
-        <f>MIN(K27,L26)+L6</f>
+        <f t="shared" si="8"/>
         <v>394</v>
       </c>
       <c r="M27" s="15">
-        <f>MIN(L27,M26)+M6</f>
+        <f t="shared" si="8"/>
         <v>412</v>
       </c>
       <c r="N27" s="15">
-        <f>MIN(M27,N26)+N6</f>
+        <f t="shared" si="8"/>
         <v>491</v>
       </c>
       <c r="O27" s="15">
-        <f>MIN(N27,O26)+O6</f>
+        <f t="shared" si="8"/>
         <v>531</v>
       </c>
       <c r="P27" s="15">
-        <f>MIN(O27,P26)+P6</f>
+        <f t="shared" si="8"/>
         <v>613</v>
       </c>
       <c r="Q27" s="15">
-        <f>MIN(P27,Q26)+Q6</f>
+        <f t="shared" si="8"/>
         <v>650</v>
       </c>
       <c r="R27" s="15">
-        <f>MIN(Q27,R26)+R6</f>
+        <f t="shared" si="8"/>
         <v>721</v>
       </c>
       <c r="S27" s="16">
-        <f>MIN(R27,S26)+S6</f>
+        <f t="shared" si="8"/>
         <v>736</v>
       </c>
       <c r="T27" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1024</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215</v>
       </c>
       <c r="B28" s="15">
-        <f>MIN(A28,B27)+B7</f>
+        <f t="shared" ref="B28:B41" si="9">MIN(A28,B27)+B7</f>
         <v>228</v>
       </c>
       <c r="C28" s="15">
-        <f>MIN(B28,C27)+C7</f>
+        <f t="shared" ref="C28:C41" si="10">MIN(B28,C27)+C7</f>
         <v>231</v>
       </c>
       <c r="D28" s="16">
-        <f>MIN(C28,D27)+D7</f>
+        <f t="shared" ref="D28:D41" si="11">MIN(C28,D27)+D7</f>
         <v>238</v>
       </c>
       <c r="E28" s="15">
@@ -2237,19 +2237,19 @@
         <v>358</v>
       </c>
       <c r="F28" s="15">
-        <f>MIN(E28,F27)+F7</f>
+        <f t="shared" ref="F28:I30" si="12">MIN(E28,F27)+F7</f>
         <v>372</v>
       </c>
       <c r="G28" s="15">
-        <f>MIN(F28,G27)+G7</f>
+        <f t="shared" si="12"/>
         <v>351</v>
       </c>
       <c r="H28" s="15">
-        <f>MIN(G28,H27)+H7</f>
+        <f t="shared" si="12"/>
         <v>358</v>
       </c>
       <c r="I28" s="15">
-        <f>MIN(H28,I27)+I7</f>
+        <f t="shared" si="12"/>
         <v>371</v>
       </c>
       <c r="J28" s="18">
@@ -2257,31 +2257,31 @@
         <v>384</v>
       </c>
       <c r="K28" s="18">
-        <f t="shared" ref="K28:N28" si="5">J28+K7</f>
+        <f t="shared" ref="K28:N28" si="13">J28+K7</f>
         <v>389</v>
       </c>
       <c r="L28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>408</v>
       </c>
       <c r="M28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>422</v>
       </c>
       <c r="N28" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>483</v>
       </c>
       <c r="O28" s="15">
-        <f>MIN(N28,O27)+O7</f>
+        <f t="shared" ref="O28:O41" si="14">MIN(N28,O27)+O7</f>
         <v>573</v>
       </c>
       <c r="P28" s="15">
-        <f>MIN(O28,P27)+P7</f>
+        <f t="shared" ref="P28:P41" si="15">MIN(O28,P27)+P7</f>
         <v>661</v>
       </c>
       <c r="Q28" s="16">
-        <f>MIN(P28,Q27)+Q7</f>
+        <f t="shared" ref="Q28:Q41" si="16">MIN(P28,Q27)+Q7</f>
         <v>698</v>
       </c>
       <c r="R28" s="15">
@@ -2289,209 +2289,209 @@
         <v>770</v>
       </c>
       <c r="S28" s="16">
-        <f>MIN(R28,S27)+S7</f>
+        <f t="shared" ref="S28:S41" si="17">MIN(R28,S27)+S7</f>
         <v>779</v>
       </c>
       <c r="T28" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1064</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>237</v>
       </c>
       <c r="B29" s="15">
-        <f>MIN(A29,B28)+B8</f>
+        <f t="shared" si="9"/>
         <v>281</v>
       </c>
       <c r="C29" s="15">
-        <f>MIN(B29,C28)+C8</f>
+        <f t="shared" si="10"/>
         <v>262</v>
       </c>
       <c r="D29" s="16">
-        <f>MIN(C29,D28)+D8</f>
+        <f t="shared" si="11"/>
         <v>302</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" ref="E29:E35" si="6">E28+E8</f>
+        <f t="shared" ref="E29:E35" si="18">E28+E8</f>
         <v>404</v>
       </c>
       <c r="F29" s="15">
-        <f>MIN(E29,F28)+F8</f>
+        <f t="shared" si="12"/>
         <v>393</v>
       </c>
       <c r="G29" s="15">
-        <f>MIN(F29,G28)+G8</f>
+        <f t="shared" si="12"/>
         <v>371</v>
       </c>
       <c r="H29" s="15">
-        <f>MIN(G29,H28)+H8</f>
+        <f t="shared" si="12"/>
         <v>371</v>
       </c>
       <c r="I29" s="15">
-        <f>MIN(H29,I28)+I8</f>
+        <f t="shared" si="12"/>
         <v>390</v>
       </c>
       <c r="J29" s="15">
-        <f>MIN(I29,J28)+J8</f>
+        <f t="shared" ref="J29:N30" si="19">MIN(I29,J28)+J8</f>
         <v>389</v>
       </c>
       <c r="K29" s="15">
-        <f>MIN(J29,K28)+K8</f>
+        <f t="shared" si="19"/>
         <v>394</v>
       </c>
       <c r="L29" s="15">
-        <f>MIN(K29,L28)+L8</f>
+        <f t="shared" si="19"/>
         <v>410</v>
       </c>
       <c r="M29" s="15">
-        <f>MIN(L29,M28)+M8</f>
+        <f t="shared" si="19"/>
         <v>415</v>
       </c>
       <c r="N29" s="15">
-        <f>MIN(M29,N28)+N8</f>
+        <f t="shared" si="19"/>
         <v>495</v>
       </c>
       <c r="O29" s="15">
-        <f>MIN(N29,O28)+O8</f>
+        <f t="shared" si="14"/>
         <v>534</v>
       </c>
       <c r="P29" s="15">
-        <f>MIN(O29,P28)+P8</f>
+        <f t="shared" si="15"/>
         <v>587</v>
       </c>
       <c r="Q29" s="16">
-        <f>MIN(P29,Q28)+Q8</f>
+        <f t="shared" si="16"/>
         <v>647</v>
       </c>
       <c r="R29" s="15">
-        <f t="shared" ref="R29:R35" si="7">R28+R8</f>
+        <f t="shared" ref="R29:R35" si="20">R28+R8</f>
         <v>839</v>
       </c>
       <c r="S29" s="16">
-        <f>MIN(R29,S28)+S8</f>
+        <f t="shared" si="17"/>
         <v>798</v>
       </c>
       <c r="T29" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1082</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
       <c r="B30" s="15">
-        <f>MIN(A30,B29)+B9</f>
+        <f t="shared" si="9"/>
         <v>331</v>
       </c>
       <c r="C30" s="15">
-        <f>MIN(B30,C29)+C9</f>
+        <f t="shared" si="10"/>
         <v>288</v>
       </c>
       <c r="D30" s="16">
-        <f>MIN(C30,D29)+D9</f>
+        <f t="shared" si="11"/>
         <v>308</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>427</v>
       </c>
       <c r="F30" s="15">
-        <f>MIN(E30,F29)+F9</f>
+        <f t="shared" si="12"/>
         <v>451</v>
       </c>
       <c r="G30" s="15">
-        <f>MIN(F30,G29)+G9</f>
+        <f t="shared" si="12"/>
         <v>386</v>
       </c>
       <c r="H30" s="15">
-        <f>MIN(G30,H29)+H9</f>
+        <f t="shared" si="12"/>
         <v>379</v>
       </c>
       <c r="I30" s="15">
-        <f>MIN(H30,I29)+I9</f>
+        <f t="shared" si="12"/>
         <v>399</v>
       </c>
       <c r="J30" s="15">
-        <f>MIN(I30,J29)+J9</f>
+        <f t="shared" si="19"/>
         <v>404</v>
       </c>
       <c r="K30" s="15">
-        <f>MIN(J30,K29)+K9</f>
+        <f t="shared" si="19"/>
         <v>401</v>
       </c>
       <c r="L30" s="15">
-        <f>MIN(K30,L29)+L9</f>
+        <f t="shared" si="19"/>
         <v>416</v>
       </c>
       <c r="M30" s="15">
-        <f>MIN(L30,M29)+M9</f>
+        <f t="shared" si="19"/>
         <v>434</v>
       </c>
       <c r="N30" s="15">
-        <f>MIN(M30,N29)+N9</f>
+        <f t="shared" si="19"/>
         <v>489</v>
       </c>
       <c r="O30" s="15">
-        <f>MIN(N30,O29)+O9</f>
+        <f t="shared" si="14"/>
         <v>583</v>
       </c>
       <c r="P30" s="15">
-        <f>MIN(O30,P29)+P9</f>
+        <f t="shared" si="15"/>
         <v>656</v>
       </c>
       <c r="Q30" s="16">
-        <f>MIN(P30,Q29)+Q9</f>
+        <f t="shared" si="16"/>
         <v>733</v>
       </c>
       <c r="R30" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>877</v>
       </c>
       <c r="S30" s="16">
-        <f>MIN(R30,S29)+S9</f>
+        <f t="shared" si="17"/>
         <v>834</v>
       </c>
       <c r="T30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1154</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>349</v>
       </c>
       <c r="B31" s="15">
-        <f>MIN(A31,B30)+B10</f>
+        <f t="shared" si="9"/>
         <v>390</v>
       </c>
       <c r="C31" s="15">
-        <f>MIN(B31,C30)+C10</f>
+        <f t="shared" si="10"/>
         <v>384</v>
       </c>
       <c r="D31" s="16">
-        <f>MIN(C31,D30)+D10</f>
+        <f t="shared" si="11"/>
         <v>381</v>
       </c>
       <c r="E31" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>473</v>
       </c>
       <c r="F31" s="15">
-        <f>MIN(E31,F30)+F10</f>
+        <f t="shared" ref="F31:F41" si="21">MIN(E31,F30)+F10</f>
         <v>497</v>
       </c>
       <c r="G31" s="15">
-        <f>MIN(F31,G30)+G10</f>
+        <f t="shared" ref="G31:G41" si="22">MIN(F31,G30)+G10</f>
         <v>398</v>
       </c>
       <c r="H31" s="16">
-        <f>MIN(G31,H30)+H10</f>
+        <f t="shared" ref="H31:H41" si="23">MIN(G31,H30)+H10</f>
         <v>388</v>
       </c>
       <c r="I31" s="15">
@@ -2499,15 +2499,15 @@
         <v>410</v>
       </c>
       <c r="J31" s="15">
-        <f>MIN(I31,J30)+J10</f>
+        <f t="shared" ref="J31:J41" si="24">MIN(I31,J30)+J10</f>
         <v>416</v>
       </c>
       <c r="K31" s="15">
-        <f>MIN(J31,K30)+K10</f>
+        <f t="shared" ref="K31:K41" si="25">MIN(J31,K30)+K10</f>
         <v>413</v>
       </c>
       <c r="L31" s="16">
-        <f>MIN(K31,L30)+L10</f>
+        <f t="shared" ref="L31:L41" si="26">MIN(K31,L30)+L10</f>
         <v>418</v>
       </c>
       <c r="M31" s="15">
@@ -2515,639 +2515,639 @@
         <v>454</v>
       </c>
       <c r="N31" s="15">
-        <f>MIN(M31,N30)+N10</f>
+        <f t="shared" ref="N31:N41" si="27">MIN(M31,N30)+N10</f>
         <v>517</v>
       </c>
       <c r="O31" s="15">
-        <f>MIN(N31,O30)+O10</f>
+        <f t="shared" si="14"/>
         <v>574</v>
       </c>
       <c r="P31" s="15">
-        <f>MIN(O31,P30)+P10</f>
+        <f t="shared" si="15"/>
         <v>593</v>
       </c>
       <c r="Q31" s="16">
-        <f>MIN(P31,Q30)+Q10</f>
+        <f t="shared" si="16"/>
         <v>670</v>
       </c>
       <c r="R31" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>950</v>
       </c>
       <c r="S31" s="15">
-        <f>MIN(R31,S30)+S10</f>
+        <f t="shared" si="17"/>
         <v>899</v>
       </c>
       <c r="T31" s="17">
-        <f>MIN(S31,T30)+T10</f>
+        <f t="shared" ref="T31:T41" si="28">MIN(S31,T30)+T10</f>
         <v>927</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>418</v>
       </c>
       <c r="B32" s="15">
-        <f>MIN(A32,B31)+B11</f>
+        <f t="shared" si="9"/>
         <v>456</v>
       </c>
       <c r="C32" s="15">
-        <f>MIN(B32,C31)+C11</f>
+        <f t="shared" si="10"/>
         <v>463</v>
       </c>
       <c r="D32" s="16">
-        <f>MIN(C32,D31)+D11</f>
+        <f t="shared" si="11"/>
         <v>426</v>
       </c>
       <c r="E32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>521</v>
       </c>
       <c r="F32" s="15">
-        <f>MIN(E32,F31)+F11</f>
+        <f t="shared" si="21"/>
         <v>512</v>
       </c>
       <c r="G32" s="15">
-        <f>MIN(F32,G31)+G11</f>
+        <f t="shared" si="22"/>
         <v>410</v>
       </c>
       <c r="H32" s="16">
-        <f>MIN(G32,H31)+H11</f>
+        <f t="shared" si="23"/>
         <v>401</v>
       </c>
       <c r="I32" s="15">
-        <f t="shared" ref="I32:I38" si="8">I31+I11</f>
+        <f t="shared" ref="I32:I38" si="29">I31+I11</f>
         <v>417</v>
       </c>
       <c r="J32" s="15">
-        <f>MIN(I32,J31)+J11</f>
+        <f t="shared" si="24"/>
         <v>428</v>
       </c>
       <c r="K32" s="15">
-        <f>MIN(J32,K31)+K11</f>
+        <f t="shared" si="25"/>
         <v>424</v>
       </c>
       <c r="L32" s="16">
-        <f>MIN(K32,L31)+L11</f>
+        <f t="shared" si="26"/>
         <v>425</v>
       </c>
       <c r="M32" s="15">
-        <f t="shared" ref="M32:M38" si="9">M31+M11</f>
+        <f t="shared" ref="M32:M38" si="30">M31+M11</f>
         <v>460</v>
       </c>
       <c r="N32" s="15">
-        <f>MIN(M32,N31)+N11</f>
+        <f t="shared" si="27"/>
         <v>529</v>
       </c>
       <c r="O32" s="15">
-        <f>MIN(N32,O31)+O11</f>
+        <f t="shared" si="14"/>
         <v>535</v>
       </c>
       <c r="P32" s="15">
-        <f>MIN(O32,P31)+P11</f>
+        <f t="shared" si="15"/>
         <v>559</v>
       </c>
       <c r="Q32" s="16">
-        <f>MIN(P32,Q31)+Q11</f>
+        <f t="shared" si="16"/>
         <v>633</v>
       </c>
       <c r="R32" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>1003</v>
       </c>
       <c r="S32" s="15">
-        <f>MIN(R32,S31)+S11</f>
+        <f t="shared" si="17"/>
         <v>930</v>
       </c>
       <c r="T32" s="17">
-        <f>MIN(S32,T31)+T11</f>
+        <f t="shared" si="28"/>
         <v>972</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>508</v>
       </c>
       <c r="B33" s="15">
-        <f>MIN(A33,B32)+B12</f>
+        <f t="shared" si="9"/>
         <v>489</v>
       </c>
       <c r="C33" s="15">
-        <f>MIN(B33,C32)+C12</f>
+        <f t="shared" si="10"/>
         <v>554</v>
       </c>
       <c r="D33" s="16">
-        <f>MIN(C33,D32)+D12</f>
+        <f t="shared" si="11"/>
         <v>489</v>
       </c>
       <c r="E33" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>568</v>
       </c>
       <c r="F33" s="15">
-        <f>MIN(E33,F32)+F12</f>
+        <f t="shared" si="21"/>
         <v>559</v>
       </c>
       <c r="G33" s="15">
-        <f>MIN(F33,G32)+G12</f>
+        <f t="shared" si="22"/>
         <v>420</v>
       </c>
       <c r="H33" s="16">
-        <f>MIN(G33,H32)+H12</f>
+        <f t="shared" si="23"/>
         <v>417</v>
       </c>
       <c r="I33" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>432</v>
       </c>
       <c r="J33" s="15">
-        <f>MIN(I33,J32)+J12</f>
+        <f t="shared" si="24"/>
         <v>442</v>
       </c>
       <c r="K33" s="15">
-        <f>MIN(J33,K32)+K12</f>
+        <f t="shared" si="25"/>
         <v>437</v>
       </c>
       <c r="L33" s="16">
-        <f>MIN(K33,L32)+L12</f>
+        <f t="shared" si="26"/>
         <v>432</v>
       </c>
       <c r="M33" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>465</v>
       </c>
       <c r="N33" s="15">
-        <f>MIN(M33,N32)+N12</f>
+        <f t="shared" si="27"/>
         <v>496</v>
       </c>
       <c r="O33" s="15">
-        <f>MIN(N33,O32)+O12</f>
+        <f t="shared" si="14"/>
         <v>541</v>
       </c>
       <c r="P33" s="15">
-        <f>MIN(O33,P32)+P12</f>
+        <f t="shared" si="15"/>
         <v>603</v>
       </c>
       <c r="Q33" s="16">
-        <f>MIN(P33,Q32)+Q12</f>
+        <f t="shared" si="16"/>
         <v>651</v>
       </c>
       <c r="R33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>1036</v>
       </c>
       <c r="S33" s="15">
-        <f>MIN(R33,S32)+S12</f>
+        <f t="shared" si="17"/>
         <v>963</v>
       </c>
       <c r="T33" s="17">
-        <f>MIN(S33,T32)+T12</f>
+        <f t="shared" si="28"/>
         <v>986</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>552</v>
       </c>
       <c r="B34" s="15">
-        <f>MIN(A34,B33)+B13</f>
+        <f t="shared" si="9"/>
         <v>547</v>
       </c>
       <c r="C34" s="15">
-        <f>MIN(B34,C33)+C13</f>
+        <f t="shared" si="10"/>
         <v>632</v>
       </c>
       <c r="D34" s="16">
-        <f>MIN(C34,D33)+D13</f>
+        <f t="shared" si="11"/>
         <v>562</v>
       </c>
       <c r="E34" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>599</v>
       </c>
       <c r="F34" s="15">
-        <f>MIN(E34,F33)+F13</f>
+        <f t="shared" si="21"/>
         <v>585</v>
       </c>
       <c r="G34" s="15">
-        <f>MIN(F34,G33)+G13</f>
+        <f t="shared" si="22"/>
         <v>429</v>
       </c>
       <c r="H34" s="16">
-        <f>MIN(G34,H33)+H13</f>
+        <f t="shared" si="23"/>
         <v>425</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>441</v>
       </c>
       <c r="J34" s="15">
-        <f>MIN(I34,J33)+J13</f>
+        <f t="shared" si="24"/>
         <v>460</v>
       </c>
       <c r="K34" s="15">
-        <f>MIN(J34,K33)+K13</f>
+        <f t="shared" si="25"/>
         <v>446</v>
       </c>
       <c r="L34" s="16">
-        <f>MIN(K34,L33)+L13</f>
+        <f t="shared" si="26"/>
         <v>442</v>
       </c>
       <c r="M34" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>478</v>
       </c>
       <c r="N34" s="15">
-        <f>MIN(M34,N33)+N13</f>
+        <f t="shared" si="27"/>
         <v>512</v>
       </c>
       <c r="O34" s="15">
-        <f>MIN(N34,O33)+O13</f>
+        <f t="shared" si="14"/>
         <v>546</v>
       </c>
       <c r="P34" s="15">
-        <f>MIN(O34,P33)+P13</f>
+        <f t="shared" si="15"/>
         <v>606</v>
       </c>
       <c r="Q34" s="16">
-        <f>MIN(P34,Q33)+Q13</f>
+        <f t="shared" si="16"/>
         <v>633</v>
       </c>
       <c r="R34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>1080</v>
       </c>
       <c r="S34" s="15">
-        <f>MIN(R34,S33)+S13</f>
+        <f t="shared" si="17"/>
         <v>992</v>
       </c>
       <c r="T34" s="17">
-        <f>MIN(S34,T33)+T13</f>
+        <f t="shared" si="28"/>
         <v>994</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>580</v>
       </c>
       <c r="B35" s="15">
-        <f>MIN(A35,B34)+B14</f>
+        <f t="shared" si="9"/>
         <v>589</v>
       </c>
       <c r="C35" s="15">
-        <f>MIN(B35,C34)+C14</f>
+        <f t="shared" si="10"/>
         <v>634</v>
       </c>
       <c r="D35" s="16">
-        <f>MIN(C35,D34)+D14</f>
+        <f t="shared" si="11"/>
         <v>617</v>
       </c>
       <c r="E35" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>649</v>
       </c>
       <c r="F35" s="15">
-        <f>MIN(E35,F34)+F14</f>
+        <f t="shared" si="21"/>
         <v>594</v>
       </c>
       <c r="G35" s="15">
-        <f>MIN(F35,G34)+G14</f>
+        <f t="shared" si="22"/>
         <v>440</v>
       </c>
       <c r="H35" s="16">
-        <f>MIN(G35,H34)+H14</f>
+        <f t="shared" si="23"/>
         <v>443</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>465</v>
       </c>
       <c r="J35" s="15">
-        <f>MIN(I35,J34)+J14</f>
+        <f t="shared" si="24"/>
         <v>472</v>
       </c>
       <c r="K35" s="15">
-        <f>MIN(J35,K34)+K14</f>
+        <f t="shared" si="25"/>
         <v>513</v>
       </c>
       <c r="L35" s="16">
-        <f>MIN(K35,L34)+L14</f>
+        <f t="shared" si="26"/>
         <v>521</v>
       </c>
       <c r="M35" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>527</v>
       </c>
       <c r="N35" s="15">
-        <f>MIN(M35,N34)+N14</f>
+        <f t="shared" si="27"/>
         <v>590</v>
       </c>
       <c r="O35" s="15">
-        <f>MIN(N35,O34)+O14</f>
+        <f t="shared" si="14"/>
         <v>597</v>
       </c>
       <c r="P35" s="15">
-        <f>MIN(O35,P34)+P14</f>
+        <f t="shared" si="15"/>
         <v>651</v>
       </c>
       <c r="Q35" s="16">
-        <f>MIN(P35,Q34)+Q14</f>
+        <f t="shared" si="16"/>
         <v>679</v>
       </c>
       <c r="R35" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>1097</v>
       </c>
       <c r="S35" s="15">
-        <f>MIN(R35,S34)+S14</f>
+        <f t="shared" si="17"/>
         <v>1033</v>
       </c>
       <c r="T35" s="17">
-        <f>MIN(S35,T34)+T14</f>
+        <f t="shared" si="28"/>
         <v>1054</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>625</v>
       </c>
       <c r="B36" s="15">
-        <f>MIN(A36,B35)+B15</f>
+        <f t="shared" si="9"/>
         <v>665</v>
       </c>
       <c r="C36" s="15">
-        <f>MIN(B36,C35)+C15</f>
+        <f t="shared" si="10"/>
         <v>724</v>
       </c>
       <c r="D36" s="15">
-        <f>MIN(C36,D35)+D15</f>
+        <f t="shared" si="11"/>
         <v>690</v>
       </c>
       <c r="E36" s="15">
-        <f>MIN(D36,E35)+E15</f>
+        <f t="shared" ref="E36:E41" si="31">MIN(D36,E35)+E15</f>
         <v>700</v>
       </c>
       <c r="F36" s="15">
-        <f>MIN(E36,F35)+F15</f>
+        <f t="shared" si="21"/>
         <v>648</v>
       </c>
       <c r="G36" s="15">
-        <f>MIN(F36,G35)+G15</f>
+        <f t="shared" si="22"/>
         <v>453</v>
       </c>
       <c r="H36" s="16">
-        <f>MIN(G36,H35)+H15</f>
+        <f t="shared" si="23"/>
         <v>520</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>514</v>
       </c>
       <c r="J36" s="15">
-        <f>MIN(I36,J35)+J15</f>
+        <f t="shared" si="24"/>
         <v>546</v>
       </c>
       <c r="K36" s="15">
-        <f>MIN(J36,K35)+K15</f>
+        <f t="shared" si="25"/>
         <v>525</v>
       </c>
       <c r="L36" s="16">
-        <f>MIN(K36,L35)+L15</f>
+        <f t="shared" si="26"/>
         <v>553</v>
       </c>
       <c r="M36" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>585</v>
       </c>
       <c r="N36" s="15">
-        <f>MIN(M36,N35)+N15</f>
+        <f t="shared" si="27"/>
         <v>602</v>
       </c>
       <c r="O36" s="15">
-        <f>MIN(N36,O35)+O15</f>
+        <f t="shared" si="14"/>
         <v>667</v>
       </c>
       <c r="P36" s="15">
-        <f>MIN(O36,P35)+P15</f>
+        <f t="shared" si="15"/>
         <v>678</v>
       </c>
       <c r="Q36" s="15">
-        <f>MIN(P36,Q35)+Q15</f>
+        <f t="shared" si="16"/>
         <v>687</v>
       </c>
       <c r="R36" s="15">
-        <f>MIN(Q36,R35)+R15</f>
+        <f t="shared" ref="R36:R41" si="32">MIN(Q36,R35)+R15</f>
         <v>767</v>
       </c>
       <c r="S36" s="15">
-        <f>MIN(R36,S35)+S15</f>
+        <f t="shared" si="17"/>
         <v>847</v>
       </c>
       <c r="T36" s="17">
-        <f>MIN(S36,T35)+T15</f>
+        <f t="shared" si="28"/>
         <v>902</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>696</v>
       </c>
       <c r="B37" s="15">
-        <f>MIN(A37,B36)+B16</f>
+        <f t="shared" si="9"/>
         <v>757</v>
       </c>
       <c r="C37" s="15">
-        <f>MIN(B37,C36)+C16</f>
+        <f t="shared" si="10"/>
         <v>757</v>
       </c>
       <c r="D37" s="15">
-        <f>MIN(C37,D36)+D16</f>
+        <f t="shared" si="11"/>
         <v>776</v>
       </c>
       <c r="E37" s="15">
-        <f>MIN(D37,E36)+E16</f>
+        <f t="shared" si="31"/>
         <v>750</v>
       </c>
       <c r="F37" s="15">
-        <f>MIN(E37,F36)+F16</f>
+        <f t="shared" si="21"/>
         <v>683</v>
       </c>
       <c r="G37" s="15">
-        <f>MIN(F37,G36)+G16</f>
+        <f t="shared" si="22"/>
         <v>467</v>
       </c>
       <c r="H37" s="16">
-        <f>MIN(G37,H36)+H16</f>
+        <f t="shared" si="23"/>
         <v>542</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>554</v>
       </c>
       <c r="J37" s="15">
-        <f>MIN(I37,J36)+J16</f>
+        <f t="shared" si="24"/>
         <v>594</v>
       </c>
       <c r="K37" s="15">
-        <f>MIN(J37,K36)+K16</f>
+        <f t="shared" si="25"/>
         <v>536</v>
       </c>
       <c r="L37" s="16">
-        <f>MIN(K37,L36)+L16</f>
+        <f t="shared" si="26"/>
         <v>587</v>
       </c>
       <c r="M37" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>600</v>
       </c>
       <c r="N37" s="15">
-        <f>MIN(M37,N36)+N16</f>
+        <f t="shared" si="27"/>
         <v>610</v>
       </c>
       <c r="O37" s="15">
-        <f>MIN(N37,O36)+O16</f>
+        <f t="shared" si="14"/>
         <v>625</v>
       </c>
       <c r="P37" s="15">
-        <f>MIN(O37,P36)+P16</f>
+        <f t="shared" si="15"/>
         <v>665</v>
       </c>
       <c r="Q37" s="15">
-        <f>MIN(P37,Q36)+Q16</f>
+        <f t="shared" si="16"/>
         <v>704</v>
       </c>
       <c r="R37" s="15">
-        <f>MIN(Q37,R36)+R16</f>
+        <f t="shared" si="32"/>
         <v>756</v>
       </c>
       <c r="S37" s="15">
-        <f>MIN(R37,S36)+S16</f>
+        <f t="shared" si="17"/>
         <v>799</v>
       </c>
       <c r="T37" s="17">
-        <f>MIN(S37,T36)+T16</f>
+        <f t="shared" si="28"/>
         <v>814</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>738</v>
       </c>
       <c r="B38" s="15">
-        <f>MIN(A38,B37)+B17</f>
+        <f t="shared" si="9"/>
         <v>831</v>
       </c>
       <c r="C38" s="15">
-        <f>MIN(B38,C37)+C17</f>
+        <f t="shared" si="10"/>
         <v>819</v>
       </c>
       <c r="D38" s="15">
-        <f>MIN(C38,D37)+D17</f>
+        <f t="shared" si="11"/>
         <v>850</v>
       </c>
       <c r="E38" s="15">
-        <f>MIN(D38,E37)+E17</f>
+        <f t="shared" si="31"/>
         <v>811</v>
       </c>
       <c r="F38" s="15">
-        <f>MIN(E38,F37)+F17</f>
+        <f t="shared" si="21"/>
         <v>753</v>
       </c>
       <c r="G38" s="15">
-        <f>MIN(F38,G37)+G17</f>
+        <f t="shared" si="22"/>
         <v>491</v>
       </c>
       <c r="H38" s="16">
-        <f>MIN(G38,H37)+H17</f>
+        <f t="shared" si="23"/>
         <v>543</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>594</v>
       </c>
       <c r="J38" s="15">
-        <f>MIN(I38,J37)+J17</f>
+        <f t="shared" si="24"/>
         <v>614</v>
       </c>
       <c r="K38" s="15">
-        <f>MIN(J38,K37)+K17</f>
+        <f t="shared" si="25"/>
         <v>551</v>
       </c>
       <c r="L38" s="16">
-        <f>MIN(K38,L37)+L17</f>
+        <f t="shared" si="26"/>
         <v>619</v>
       </c>
       <c r="M38" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>661</v>
       </c>
       <c r="N38" s="15">
-        <f>MIN(M38,N37)+N17</f>
+        <f t="shared" si="27"/>
         <v>681</v>
       </c>
       <c r="O38" s="15">
-        <f>MIN(N38,O37)+O17</f>
+        <f t="shared" si="14"/>
         <v>639</v>
       </c>
       <c r="P38" s="15">
-        <f>MIN(O38,P37)+P17</f>
+        <f t="shared" si="15"/>
         <v>699</v>
       </c>
       <c r="Q38" s="15">
-        <f>MIN(P38,Q37)+Q17</f>
+        <f t="shared" si="16"/>
         <v>722</v>
       </c>
       <c r="R38" s="15">
-        <f>MIN(Q38,R37)+R17</f>
+        <f t="shared" si="32"/>
         <v>784</v>
       </c>
       <c r="S38" s="15">
-        <f>MIN(R38,S37)+S17</f>
+        <f t="shared" si="17"/>
         <v>802</v>
       </c>
       <c r="T38" s="17">
-        <f>MIN(S38,T37)+T17</f>
+        <f t="shared" si="28"/>
         <v>880</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>783</v>
       </c>
       <c r="B39" s="15">
-        <f>MIN(A39,B38)+B18</f>
+        <f t="shared" si="9"/>
         <v>842</v>
       </c>
       <c r="C39" s="15">
-        <f>MIN(B39,C38)+C18</f>
+        <f t="shared" si="10"/>
         <v>852</v>
       </c>
       <c r="D39" s="15">
-        <f>MIN(C39,D38)+D18</f>
+        <f t="shared" si="11"/>
         <v>923</v>
       </c>
       <c r="E39" s="15">
-        <f>MIN(D39,E38)+E18</f>
+        <f t="shared" si="31"/>
         <v>892</v>
       </c>
       <c r="F39" s="15">
-        <f>MIN(E39,F38)+F18</f>
+        <f t="shared" si="21"/>
         <v>787</v>
       </c>
       <c r="G39" s="15">
-        <f>MIN(F39,G38)+G18</f>
+        <f t="shared" si="22"/>
         <v>516</v>
       </c>
       <c r="H39" s="15">
-        <f>MIN(G39,H38)+H18</f>
+        <f t="shared" si="23"/>
         <v>588</v>
       </c>
       <c r="I39" s="15">
@@ -3155,15 +3155,15 @@
         <v>593</v>
       </c>
       <c r="J39" s="15">
-        <f>MIN(I39,J38)+J18</f>
+        <f t="shared" si="24"/>
         <v>631</v>
       </c>
       <c r="K39" s="15">
-        <f>MIN(J39,K38)+K18</f>
+        <f t="shared" si="25"/>
         <v>596</v>
       </c>
       <c r="L39" s="15">
-        <f>MIN(K39,L38)+L18</f>
+        <f t="shared" si="26"/>
         <v>607</v>
       </c>
       <c r="M39" s="15">
@@ -3171,65 +3171,65 @@
         <v>643</v>
       </c>
       <c r="N39" s="15">
-        <f>MIN(M39,N38)+N18</f>
+        <f t="shared" si="27"/>
         <v>711</v>
       </c>
       <c r="O39" s="15">
-        <f>MIN(N39,O38)+O18</f>
+        <f t="shared" si="14"/>
         <v>679</v>
       </c>
       <c r="P39" s="15">
-        <f>MIN(O39,P38)+P18</f>
+        <f t="shared" si="15"/>
         <v>707</v>
       </c>
       <c r="Q39" s="15">
-        <f>MIN(P39,Q38)+Q18</f>
+        <f t="shared" si="16"/>
         <v>779</v>
       </c>
       <c r="R39" s="15">
-        <f>MIN(Q39,R38)+R18</f>
+        <f t="shared" si="32"/>
         <v>828</v>
       </c>
       <c r="S39" s="15">
-        <f>MIN(R39,S38)+S18</f>
+        <f t="shared" si="17"/>
         <v>866</v>
       </c>
       <c r="T39" s="17">
-        <f>MIN(S39,T38)+T18</f>
+        <f t="shared" si="28"/>
         <v>924</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>851</v>
       </c>
       <c r="B40" s="15">
-        <f>MIN(A40,B39)+B19</f>
+        <f t="shared" si="9"/>
         <v>874</v>
       </c>
       <c r="C40" s="15">
-        <f>MIN(B40,C39)+C19</f>
+        <f t="shared" si="10"/>
         <v>900</v>
       </c>
       <c r="D40" s="15">
-        <f>MIN(C40,D39)+D19</f>
+        <f t="shared" si="11"/>
         <v>934</v>
       </c>
       <c r="E40" s="15">
-        <f>MIN(D40,E39)+E19</f>
+        <f t="shared" si="31"/>
         <v>931</v>
       </c>
       <c r="F40" s="15">
-        <f>MIN(E40,F39)+F19</f>
+        <f t="shared" si="21"/>
         <v>818</v>
       </c>
       <c r="G40" s="15">
-        <f>MIN(F40,G39)+G19</f>
+        <f t="shared" si="22"/>
         <v>546</v>
       </c>
       <c r="H40" s="15">
-        <f>MIN(G40,H39)+H19</f>
+        <f t="shared" si="23"/>
         <v>608</v>
       </c>
       <c r="I40" s="15">
@@ -3237,15 +3237,15 @@
         <v>606</v>
       </c>
       <c r="J40" s="15">
-        <f>MIN(I40,J39)+J19</f>
+        <f t="shared" si="24"/>
         <v>642</v>
       </c>
       <c r="K40" s="15">
-        <f>MIN(J40,K39)+K19</f>
+        <f t="shared" si="25"/>
         <v>635</v>
       </c>
       <c r="L40" s="15">
-        <f>MIN(K40,L39)+L19</f>
+        <f t="shared" si="26"/>
         <v>669</v>
       </c>
       <c r="M40" s="15">
@@ -3253,62 +3253,62 @@
         <v>674</v>
       </c>
       <c r="N40" s="15">
-        <f>MIN(M40,N39)+N19</f>
+        <f t="shared" si="27"/>
         <v>754</v>
       </c>
       <c r="O40" s="15">
-        <f>MIN(N40,O39)+O19</f>
+        <f t="shared" si="14"/>
         <v>735</v>
       </c>
       <c r="P40" s="15">
-        <f>MIN(O40,P39)+P19</f>
+        <f t="shared" si="15"/>
         <v>757</v>
       </c>
       <c r="Q40" s="15">
-        <f>MIN(P40,Q39)+Q19</f>
+        <f t="shared" si="16"/>
         <v>793</v>
       </c>
       <c r="R40" s="15">
-        <f>MIN(Q40,R39)+R19</f>
+        <f t="shared" si="32"/>
         <v>844</v>
       </c>
       <c r="S40" s="15">
-        <f>MIN(R40,S39)+S19</f>
+        <f t="shared" si="17"/>
         <v>917</v>
       </c>
       <c r="T40" s="17">
-        <f>MIN(S40,T39)+T19</f>
+        <f t="shared" si="28"/>
         <v>984</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" s="20">
-        <f>MIN(A41,B40)+B20</f>
+        <f t="shared" si="9"/>
         <v>969</v>
       </c>
       <c r="C41" s="20">
-        <f>MIN(B41,C40)+C20</f>
+        <f t="shared" si="10"/>
         <v>944</v>
       </c>
       <c r="D41" s="20">
-        <f>MIN(C41,D40)+D20</f>
+        <f t="shared" si="11"/>
         <v>970</v>
       </c>
       <c r="E41" s="20">
-        <f>MIN(D41,E40)+E20</f>
+        <f t="shared" si="31"/>
         <v>990</v>
       </c>
       <c r="F41" s="20">
-        <f>MIN(E41,F40)+F20</f>
+        <f t="shared" si="21"/>
         <v>825</v>
       </c>
       <c r="G41" s="20">
-        <f>MIN(F41,G40)+G20</f>
+        <f t="shared" si="22"/>
         <v>621</v>
       </c>
       <c r="H41" s="20">
-        <f>MIN(G41,H40)+H20</f>
+        <f t="shared" si="23"/>
         <v>680</v>
       </c>
       <c r="I41" s="20">
@@ -3316,15 +3316,15 @@
         <v>638</v>
       </c>
       <c r="J41" s="20">
-        <f>MIN(I41,J40)+J20</f>
+        <f t="shared" si="24"/>
         <v>709</v>
       </c>
       <c r="K41" s="20">
-        <f>MIN(J41,K40)+K20</f>
+        <f t="shared" si="25"/>
         <v>672</v>
       </c>
       <c r="L41" s="20">
-        <f>MIN(K41,L40)+L20</f>
+        <f t="shared" si="26"/>
         <v>724</v>
       </c>
       <c r="M41" s="20">
@@ -3332,31 +3332,31 @@
         <v>701</v>
       </c>
       <c r="N41" s="20">
-        <f>MIN(M41,N40)+N20</f>
+        <f t="shared" si="27"/>
         <v>746</v>
       </c>
       <c r="O41" s="20">
-        <f>MIN(N41,O40)+O20</f>
+        <f t="shared" si="14"/>
         <v>802</v>
       </c>
       <c r="P41" s="20">
-        <f>MIN(O41,P40)+P20</f>
+        <f t="shared" si="15"/>
         <v>793</v>
       </c>
       <c r="Q41" s="20">
-        <f>MIN(P41,Q40)+Q20</f>
+        <f t="shared" si="16"/>
         <v>843</v>
       </c>
       <c r="R41" s="20">
-        <f>MIN(Q41,R40)+R20</f>
+        <f t="shared" si="32"/>
         <v>873</v>
       </c>
       <c r="S41" s="20">
-        <f>MIN(R41,S40)+S20</f>
+        <f t="shared" si="17"/>
         <v>891</v>
       </c>
       <c r="T41" s="21">
-        <f>MIN(S41,T40)+T20</f>
+        <f t="shared" si="28"/>
         <v>902</v>
       </c>
     </row>

</xml_diff>